<commit_message>
Comecei o Felipe Neto 1
</commit_message>
<xml_diff>
--- a/Felipe Neto1(set).xlsx
+++ b/Felipe Neto1(set).xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erick.LAPTOP-MLIJ069K\Desktop\Insper\Ciência dos Dados\Projeto_2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB34A3A-DDC0-4940-8DB2-B0FE6FF3DE82}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
     <sheet name="Teste" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -594,8 +600,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -658,6 +664,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -704,7 +718,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -736,9 +750,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -770,6 +802,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -945,1514 +995,1690 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A301"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="202" spans="1:1">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:1">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="204" spans="1:1">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:1">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:1">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="207" spans="1:1">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="208" spans="1:1">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:1">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="210" spans="1:1">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:1">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="212" spans="1:1">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="213" spans="1:1">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="214" spans="1:1">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="215" spans="1:1">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:1">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="217" spans="1:1">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="218" spans="1:1">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="219" spans="1:1">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="220" spans="1:1">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="221" spans="1:1">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="222" spans="1:1">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:1">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="224" spans="1:1">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="225" spans="1:1">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="226" spans="1:1">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="227" spans="1:1">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="228" spans="1:1">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="1:1">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="230" spans="1:1">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="231" spans="1:1">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="232" spans="1:1">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="233" spans="1:1">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="234" spans="1:1">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="235" spans="1:1">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:1">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="237" spans="1:1">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="238" spans="1:1">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="239" spans="1:1">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="240" spans="1:1">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="241" spans="1:1">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="242" spans="1:1">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="243" spans="1:1">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="244" spans="1:1">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="245" spans="1:1">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="246" spans="1:1">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="247" spans="1:1">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="248" spans="1:1">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:1">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="250" spans="1:1">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="251" spans="1:1">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="252" spans="1:1">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="253" spans="1:1">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="254" spans="1:1">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="255" spans="1:1">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="256" spans="1:1">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:1">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:1">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="259" spans="1:1">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="260" spans="1:1">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="261" spans="1:1">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="262" spans="1:1">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="263" spans="1:1">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="264" spans="1:1">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="265" spans="1:1">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="266" spans="1:1">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="267" spans="1:1">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="268" spans="1:1">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="269" spans="1:1">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="270" spans="1:1">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="271" spans="1:1">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="272" spans="1:1">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:1">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="274" spans="1:1">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="275" spans="1:1">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="276" spans="1:1">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="277" spans="1:1">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="278" spans="1:1">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="279" spans="1:1">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="280" spans="1:1">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="281" spans="1:1">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="282" spans="1:1">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="283" spans="1:1">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="284" spans="1:1">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="1:1">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="286" spans="1:1">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:1">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="288" spans="1:1">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="289" spans="1:1">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="290" spans="1:1">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="291" spans="1:1">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="292" spans="1:1">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="293" spans="1:1">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="294" spans="1:1">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="295" spans="1:1">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="296" spans="1:1">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="297" spans="1:1">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="298" spans="1:1">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="299" spans="1:1">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="300" spans="1:1">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="301" spans="1:1">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>10</v>
       </c>
@@ -2463,1014 +2689,1014 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A201"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>45</v>
       </c>

</xml_diff>